<commit_message>
chore: Documentation updates, audit reports, backend tests, config, reference data
Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/reference/multifam/chadron/Chadron - Rent Roll & Delinquency 09.30.2025.xlsx
+++ b/reference/multifam/chadron/Chadron - Rent Roll & Delinquency 09.30.2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/5150east/landscape/reference/multifam/chadron/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E81637-97D3-4E49-908D-A2167B0F3D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCECBA8C-3B80-734C-BE87-E66EF7F63A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="4740" windowWidth="24780" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1321,7 +1321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1418,6 +1418,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1740,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R134"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2193,7 +2194,7 @@
       <c r="G17" s="5">
         <v>1700</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="46">
         <v>44562</v>
       </c>
       <c r="I17" s="7">

</xml_diff>